<commit_message>
Experiments and minor fixes
</commit_message>
<xml_diff>
--- a/Experiments/comparison.xlsx
+++ b/Experiments/comparison.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="168">
   <si>
     <t>Comparison of models</t>
   </si>
@@ -509,6 +509,18 @@
   </si>
   <si>
     <t>119 (117.932, 120.100)</t>
+  </si>
+  <si>
+    <t>esn: 256, ro:32</t>
+  </si>
+  <si>
+    <t>1603.96</t>
+  </si>
+  <si>
+    <t>126.83</t>
+  </si>
+  <si>
+    <t>123.164 (117.384, 117.688)</t>
   </si>
 </sst>
 </file>
@@ -2481,7 +2493,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="A26" sqref="A26:N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3304,12 +3316,12 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="7" max="7" width="7.42578125" customWidth="1"/>
@@ -3983,7 +3995,7 @@
       <c r="P20" s="17"/>
       <c r="Q20" s="17"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
@@ -4002,45 +4014,85 @@
       <c r="P21" s="17"/>
       <c r="Q21" s="17"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
+    <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
+      <c r="F22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="M22" s="35" t="s">
+        <v>98</v>
+      </c>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="17"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
+      <c r="A23" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="14">
+        <v>20</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="14">
+        <v>850</v>
+      </c>
+      <c r="G23" s="14">
+        <v>2</v>
+      </c>
+      <c r="H23" s="14">
+        <v>0</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="L23" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>167</v>
+      </c>
       <c r="N23" s="17"/>
       <c r="O23" s="17"/>
       <c r="P23" s="17"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
-        <v>152</v>
-      </c>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -4058,9 +4110,6 @@
       <c r="P24" s="17"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
-        <v>139</v>
-      </c>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -4096,7 +4145,9 @@
       <c r="P26" s="17"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="17"/>
+      <c r="A27" s="17" t="s">
+        <v>152</v>
+      </c>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -4114,7 +4165,9 @@
       <c r="P27" s="17"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+      <c r="A28" s="17" t="s">
+        <v>139</v>
+      </c>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -4150,7 +4203,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4159,6 +4212,7 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="6.85546875" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="11" max="11" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4203,262 +4257,298 @@
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="29" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8" s="22"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E9" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30" t="s">
+      <c r="F9" s="46"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="22"/>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="G10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J10" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K10" s="12" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B11" s="14">
         <v>10</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C11" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D11" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E11" s="14">
         <v>100</v>
       </c>
-      <c r="F8" s="14">
-        <v>0</v>
-      </c>
-      <c r="G8" s="14">
+      <c r="F11" s="14">
+        <v>0</v>
+      </c>
+      <c r="G11" s="14">
         <v>2</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="14">
+      <c r="I11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="14">
         <v>64</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K11" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="22"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B12" s="19">
         <v>10</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C12" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D12" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E12" s="19">
         <v>400</v>
       </c>
-      <c r="F9" s="19">
-        <v>0</v>
-      </c>
-      <c r="G9" s="19">
+      <c r="F12" s="19">
+        <v>0</v>
+      </c>
+      <c r="G12" s="19">
         <v>2</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H12" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="19" t="s">
+      <c r="I12" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K12" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="L9" s="22"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B13" s="19">
         <v>20</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C13" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D13" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E13" s="19">
         <v>160</v>
       </c>
-      <c r="F10" s="19">
-        <v>0</v>
-      </c>
-      <c r="G10" s="19">
-        <v>5</v>
-      </c>
-      <c r="H10" s="19" t="s">
+      <c r="F13" s="19">
+        <v>0</v>
+      </c>
+      <c r="G13" s="19">
+        <v>5</v>
+      </c>
+      <c r="H13" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="19" t="s">
+      <c r="I13" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K13" s="19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B14" s="19">
+        <v>15</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="19">
+        <v>520</v>
+      </c>
+      <c r="F14" s="19">
+        <v>0</v>
+      </c>
+      <c r="G14" s="19">
+        <v>2</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="G18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="J18" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="K18" s="12" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="L18" s="17"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B19" s="14">
         <v>20</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C19" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14">
+      <c r="D19" s="14"/>
+      <c r="E19" s="14">
         <v>460</v>
       </c>
-      <c r="F16" s="14">
-        <v>0</v>
-      </c>
-      <c r="G16" s="14">
-        <v>5</v>
-      </c>
-      <c r="H16" s="14" t="s">
+      <c r="F19" s="14">
+        <v>0</v>
+      </c>
+      <c r="G19" s="14">
+        <v>5</v>
+      </c>
+      <c r="H19" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="14" t="s">
+      <c r="I19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="14" t="s">
+      <c r="K19" s="14" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
       <c r="L19" s="17"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -4472,11 +4562,13 @@
       <c r="L20" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
-    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Visualizations + minor fixes and changes
</commit_message>
<xml_diff>
--- a/Experiments/comparison.xlsx
+++ b/Experiments/comparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="2048" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="152">
   <si>
     <t>Comparison of models</t>
   </si>
@@ -49,54 +49,21 @@
     <t>relu</t>
   </si>
   <si>
-    <t>0.01, 0.5</t>
-  </si>
-  <si>
     <t>xover</t>
   </si>
   <si>
     <t>uniform, 0.1, 0.1</t>
   </si>
   <si>
-    <t>3057.47</t>
-  </si>
-  <si>
-    <t>2973.74</t>
-  </si>
-  <si>
-    <t>2989.58</t>
-  </si>
-  <si>
-    <t>uniform, 0.3, 0.1</t>
-  </si>
-  <si>
-    <t>3018.47</t>
-  </si>
-  <si>
     <t>uniform, 0.05, 0.1</t>
   </si>
   <si>
-    <t>3034.74</t>
-  </si>
-  <si>
-    <t>3091.59</t>
-  </si>
-  <si>
     <t>selbest</t>
   </si>
   <si>
     <t>0.2, 0.5</t>
   </si>
   <si>
-    <t>3125.42</t>
-  </si>
-  <si>
-    <t>tanh</t>
-  </si>
-  <si>
-    <t>2980.13</t>
-  </si>
-  <si>
     <t>MARIO</t>
   </si>
   <si>
@@ -106,9 +73,6 @@
     <t>TORCS</t>
   </si>
   <si>
-    <t>3195.75</t>
-  </si>
-  <si>
     <t>120.44</t>
   </si>
   <si>
@@ -118,9 +82,6 @@
     <t>4x64</t>
   </si>
   <si>
-    <t>2788.45</t>
-  </si>
-  <si>
     <t>0.92</t>
   </si>
   <si>
@@ -139,12 +100,6 @@
     <t>0.96</t>
   </si>
   <si>
-    <t>0.75, 0.5</t>
-  </si>
-  <si>
-    <t>3115.12</t>
-  </si>
-  <si>
     <t>0.5, 0.1</t>
   </si>
   <si>
@@ -160,9 +115,6 @@
     <t>82.39% (206/250)</t>
   </si>
   <si>
-    <t>2915.33</t>
-  </si>
-  <si>
     <t>CMA-ES</t>
   </si>
   <si>
@@ -178,12 +130,6 @@
     <t>3 players</t>
   </si>
   <si>
-    <t>uniform 0.05, 0.1</t>
-  </si>
-  <si>
-    <t>2790.05</t>
-  </si>
-  <si>
     <t>0.5, 0.2</t>
   </si>
   <si>
@@ -229,9 +175,6 @@
     <t>['119.77', '113.98', '118.1']</t>
   </si>
   <si>
-    <t>0.75, 0.3</t>
-  </si>
-  <si>
     <t>solver type</t>
   </si>
   <si>
@@ -241,15 +184,9 @@
     <t>game batch</t>
   </si>
   <si>
-    <t>128, 64, 32</t>
-  </si>
-  <si>
     <t>Best AVG Fitness</t>
   </si>
   <si>
-    <t>3205.66</t>
-  </si>
-  <si>
     <t>sigma</t>
   </si>
   <si>
@@ -319,27 +256,9 @@
     <t>['112.48', '119.44', '117.92']</t>
   </si>
   <si>
-    <t>2857.33</t>
-  </si>
-  <si>
-    <t>2764.11</t>
-  </si>
-  <si>
     <t>133.78</t>
   </si>
   <si>
-    <t>0.5, 0.3</t>
-  </si>
-  <si>
-    <t>uniform 0.3, 0.1</t>
-  </si>
-  <si>
-    <t>5851.63</t>
-  </si>
-  <si>
-    <t>5848.18</t>
-  </si>
-  <si>
     <t>MLP</t>
   </si>
   <si>
@@ -367,33 +286,12 @@
     <t>130.41</t>
   </si>
   <si>
-    <t>uniform 0.1, 0.1</t>
-  </si>
-  <si>
     <t>512, 512</t>
   </si>
   <si>
-    <t>5845.06</t>
-  </si>
-  <si>
-    <t>5846.07</t>
-  </si>
-  <si>
-    <t>256, 256</t>
-  </si>
-  <si>
     <t>inputs scale</t>
   </si>
   <si>
-    <t>div 2048</t>
-  </si>
-  <si>
-    <t>3314.26</t>
-  </si>
-  <si>
-    <t>log(x) or 0</t>
-  </si>
-  <si>
     <t>SEA+ESN</t>
   </si>
   <si>
@@ -412,15 +310,6 @@
     <t>esn:256, ro:32</t>
   </si>
   <si>
-    <t>4347.37</t>
-  </si>
-  <si>
-    <t>Random: 1077.92</t>
-  </si>
-  <si>
-    <t>Random: 82.66**</t>
-  </si>
-  <si>
     <t>** notice that the Alhambra "model" within the game is still the same (rule system has just random "weights")</t>
   </si>
   <si>
@@ -430,27 +319,12 @@
     <t>↑ There was a bug within the game phases, causing that individual weights were shared amongst phases (all phases used first 'n' values); leaving results here just for compare</t>
   </si>
   <si>
-    <t>Random: 6.016</t>
-  </si>
-  <si>
     <t>Individual length = dimension of centroid to optimize</t>
   </si>
   <si>
-    <t>4378.98</t>
-  </si>
-  <si>
     <t>CMA-ES+ESN</t>
   </si>
   <si>
-    <t>3912.66</t>
-  </si>
-  <si>
-    <t>5.0</t>
-  </si>
-  <si>
-    <t>4358.49</t>
-  </si>
-  <si>
     <t>84.39% (211/250)</t>
   </si>
   <si>
@@ -475,12 +349,6 @@
     <t>Due to many game phases (12) within the Alhambra game, the mlp - individual to evolve is too big for evolution strategy</t>
   </si>
   <si>
-    <t>uniform, 0.01, 0.1</t>
-  </si>
-  <si>
-    <t>3478.38</t>
-  </si>
-  <si>
     <t>ens:256, ro:32</t>
   </si>
   <si>
@@ -511,21 +379,12 @@
     <t>esn: 256, ro:32</t>
   </si>
   <si>
-    <t>1603.96</t>
-  </si>
-  <si>
     <t>126.83</t>
   </si>
   <si>
     <t>123.164 (117.384, 117.688)</t>
   </si>
   <si>
-    <t>esn: 128, ro:16</t>
-  </si>
-  <si>
-    <t>5851.70</t>
-  </si>
-  <si>
     <t>DE+MLP</t>
   </si>
   <si>
@@ -544,24 +403,15 @@
     <t>0.25</t>
   </si>
   <si>
-    <t>2845.13</t>
-  </si>
-  <si>
     <t>evaluation*</t>
   </si>
   <si>
     <t>* We tried two types of evaluating individuals, partial = evaluating fitness only in changed invididuals in population; full = evaluating all individuals in population</t>
   </si>
   <si>
-    <t>full</t>
-  </si>
-  <si>
     <t>partial</t>
   </si>
   <si>
-    <t>4230.35</t>
-  </si>
-  <si>
     <t>137.37</t>
   </si>
   <si>
@@ -577,13 +427,52 @@
     <t>0.91</t>
   </si>
   <si>
-    <t>Random: 0.04511 (Gomba)</t>
-  </si>
-  <si>
     <t>65.59% (164/250)</t>
   </si>
   <si>
     <t>67.60% (169/250)</t>
+  </si>
+  <si>
+    <t>Random: 1100.42</t>
+  </si>
+  <si>
+    <t>--GAME 2048 STATISTICS--</t>
+  </si>
+  <si>
+    <t>Model: random</t>
+  </si>
+  <si>
+    <t>Total games: 10000, Average score: 1100.828, Average moves: 118.7604</t>
+  </si>
+  <si>
+    <t>Reached tiles:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   16:    23 =  0.23%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   32:   648 =  6.48%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   64:  3762 = 37.62%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  128:  4739 = 47.39%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  256:   826 =  8.26%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  512:     2 =  0.02%</t>
+  </si>
+  <si>
+    <t>Random: 80.47**</t>
+  </si>
+  <si>
+    <t>Random: 0.047 (Gomba)</t>
+  </si>
+  <si>
+    <t>Random: 0.01</t>
   </si>
 </sst>
 </file>
@@ -660,7 +549,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -973,11 +862,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1119,6 +1079,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1138,6 +1104,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1150,14 +1119,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1466,10 +1449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R111"/>
+  <dimension ref="A1:U111"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1486,80 +1469,80 @@
     <col min="13" max="13" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>171</v>
-      </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-    </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+    </row>
+    <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>0</v>
       </c>
@@ -1568,10 +1551,10 @@
       <c r="D9" s="11">
         <v>2048</v>
       </c>
-      <c r="E9" s="51" t="s">
-        <v>132</v>
-      </c>
-      <c r="F9" s="52"/>
+      <c r="E9" s="53" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="54"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -1579,15 +1562,15 @@
       <c r="K9" s="23"/>
       <c r="L9" s="8"/>
     </row>
-    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>2</v>
@@ -1608,759 +1591,529 @@
         <v>7</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="K10" s="32" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="L10" s="24" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="M10" s="36" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="O10" s="63" t="s">
+        <v>139</v>
+      </c>
+      <c r="P10" s="64"/>
+      <c r="Q10" s="65"/>
+      <c r="R10" s="65"/>
+      <c r="S10" s="65"/>
+      <c r="T10" s="66"/>
+      <c r="U10" s="67"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B11" s="13">
         <v>50</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="14">
-        <v>200</v>
-      </c>
-      <c r="F11" s="14">
-        <v>0</v>
-      </c>
-      <c r="G11" s="14">
-        <v>5</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="15">
-        <v>16</v>
-      </c>
-      <c r="K11" s="15">
-        <v>10</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="M11" s="37" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="37"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="69"/>
+      <c r="Q11" s="70"/>
+      <c r="R11" s="70"/>
+      <c r="S11" s="70"/>
+      <c r="T11" s="71"/>
+      <c r="U11" s="72"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B12" s="13">
         <v>50</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="14">
-        <v>200</v>
-      </c>
-      <c r="F12" s="14">
-        <v>0</v>
-      </c>
-      <c r="G12" s="14">
-        <v>5</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="15">
-        <v>64</v>
-      </c>
-      <c r="K12" s="20">
-        <v>10</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="M12" s="37" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="37"/>
+      <c r="O12" s="68" t="s">
+        <v>140</v>
+      </c>
+      <c r="P12" s="69"/>
+      <c r="Q12" s="70"/>
+      <c r="R12" s="70"/>
+      <c r="S12" s="70"/>
+      <c r="T12" s="71"/>
+      <c r="U12" s="72"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B13" s="13">
         <v>50</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="14">
-        <v>200</v>
-      </c>
-      <c r="F13" s="14">
-        <v>0</v>
-      </c>
-      <c r="G13" s="14">
-        <v>5</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="15">
-        <v>16</v>
-      </c>
-      <c r="K13" s="20">
-        <v>10</v>
-      </c>
-      <c r="L13" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="M13" s="37" t="s">
-        <v>122</v>
-      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="37"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O13" s="68"/>
+      <c r="P13" s="69"/>
+      <c r="Q13" s="70"/>
+      <c r="R13" s="70"/>
+      <c r="S13" s="70"/>
+      <c r="T13" s="71"/>
+      <c r="U13" s="72"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B14" s="13">
         <v>50</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="14">
-        <v>200</v>
-      </c>
-      <c r="F14" s="14">
-        <v>0</v>
-      </c>
-      <c r="G14" s="14">
-        <v>5</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" s="15">
-        <v>16</v>
-      </c>
-      <c r="K14" s="20">
-        <v>10</v>
-      </c>
-      <c r="L14" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="M14" s="37" t="s">
-        <v>122</v>
-      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="37"/>
       <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O14" s="68" t="s">
+        <v>141</v>
+      </c>
+      <c r="P14" s="69"/>
+      <c r="Q14" s="70"/>
+      <c r="R14" s="70"/>
+      <c r="S14" s="70"/>
+      <c r="T14" s="71"/>
+      <c r="U14" s="72"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B15" s="13">
         <v>50</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="14">
-        <v>200</v>
-      </c>
-      <c r="F15" s="14">
-        <v>5</v>
-      </c>
-      <c r="G15" s="14">
-        <v>0</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="15">
-        <v>16</v>
-      </c>
-      <c r="K15" s="20">
-        <v>10</v>
-      </c>
-      <c r="L15" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="37" t="s">
-        <v>122</v>
-      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="37"/>
       <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O15" s="68"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="70"/>
+      <c r="R15" s="70"/>
+      <c r="S15" s="70"/>
+      <c r="T15" s="71"/>
+      <c r="U15" s="72"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B16" s="13">
         <v>50</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="14">
-        <v>200</v>
-      </c>
-      <c r="F16" s="14">
-        <v>0</v>
-      </c>
-      <c r="G16" s="14">
-        <v>5</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="15">
-        <v>16</v>
-      </c>
-      <c r="K16" s="20">
-        <v>10</v>
-      </c>
-      <c r="L16" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="M16" s="37" t="s">
-        <v>122</v>
-      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="37"/>
       <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O16" s="68" t="s">
+        <v>142</v>
+      </c>
+      <c r="P16" s="69"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="70"/>
+      <c r="S16" s="70"/>
+      <c r="T16" s="71"/>
+      <c r="U16" s="72"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B17" s="18">
         <v>50</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="19">
-        <v>200</v>
-      </c>
-      <c r="F17" s="19">
-        <v>0</v>
-      </c>
-      <c r="G17" s="19">
-        <v>5</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J17" s="20">
-        <v>16</v>
-      </c>
-      <c r="K17" s="20">
-        <v>10</v>
-      </c>
-      <c r="L17" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M17" s="37" t="s">
-        <v>122</v>
-      </c>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="37"/>
       <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O17" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="P17" s="69"/>
+      <c r="Q17" s="70"/>
+      <c r="R17" s="70"/>
+      <c r="S17" s="70"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="72"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B18" s="18">
         <v>50</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="19">
-        <v>200</v>
-      </c>
-      <c r="F18" s="19">
-        <v>0</v>
-      </c>
-      <c r="G18" s="19">
-        <v>5</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="J18" s="20">
-        <v>16</v>
-      </c>
-      <c r="K18" s="20">
-        <v>10</v>
-      </c>
-      <c r="L18" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="M18" s="37" t="s">
-        <v>122</v>
-      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="37"/>
       <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O18" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="P18" s="69"/>
+      <c r="Q18" s="70"/>
+      <c r="R18" s="70"/>
+      <c r="S18" s="70"/>
+      <c r="T18" s="71"/>
+      <c r="U18" s="72"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B19" s="18">
         <v>50</v>
       </c>
-      <c r="C19" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="19">
-        <v>1000</v>
-      </c>
-      <c r="F19" s="19">
-        <v>0</v>
-      </c>
-      <c r="G19" s="19">
-        <v>5</v>
-      </c>
-      <c r="H19" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="20">
-        <v>16</v>
-      </c>
-      <c r="K19" s="20">
-        <v>10</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="M19" s="37" t="s">
-        <v>122</v>
-      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="37"/>
       <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O19" s="68" t="s">
+        <v>145</v>
+      </c>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="70"/>
+      <c r="R19" s="70"/>
+      <c r="S19" s="70"/>
+      <c r="T19" s="71"/>
+      <c r="U19" s="72"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B20" s="18">
         <v>25</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="19">
-        <v>200</v>
-      </c>
-      <c r="F20" s="19">
-        <v>0</v>
-      </c>
-      <c r="G20" s="19">
-        <v>5</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="K20" s="20">
-        <v>5</v>
-      </c>
-      <c r="L20" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="M20" s="37" t="s">
-        <v>122</v>
-      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="37"/>
       <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O20" s="68" t="s">
+        <v>146</v>
+      </c>
+      <c r="P20" s="69"/>
+      <c r="Q20" s="70"/>
+      <c r="R20" s="70"/>
+      <c r="S20" s="70"/>
+      <c r="T20" s="71"/>
+      <c r="U20" s="72"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B21" s="18">
         <v>50</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="19">
-        <v>140</v>
-      </c>
-      <c r="F21" s="18">
-        <v>0</v>
-      </c>
-      <c r="G21" s="19">
-        <v>5</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I21" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="K21" s="20">
-        <v>10</v>
-      </c>
-      <c r="L21" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="M21" s="37" t="s">
-        <v>122</v>
-      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="37"/>
       <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O21" s="73" t="s">
+        <v>147</v>
+      </c>
+      <c r="P21" s="74"/>
+      <c r="Q21" s="70"/>
+      <c r="R21" s="70"/>
+      <c r="S21" s="70"/>
+      <c r="T21" s="71"/>
+      <c r="U21" s="72"/>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B22" s="18">
         <v>50</v>
       </c>
-      <c r="C22" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="19">
-        <v>320</v>
-      </c>
-      <c r="F22" s="19">
-        <v>0</v>
-      </c>
-      <c r="G22" s="19">
-        <v>5</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="K22" s="20">
-        <v>5</v>
-      </c>
-      <c r="L22" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="M22" s="37" t="s">
-        <v>122</v>
-      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="37"/>
       <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O22" s="75" t="s">
+        <v>148</v>
+      </c>
+      <c r="P22" s="76"/>
+      <c r="Q22" s="79"/>
+      <c r="R22" s="79"/>
+      <c r="S22" s="79"/>
+      <c r="T22" s="77"/>
+      <c r="U22" s="78"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B23" s="18">
         <v>50</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="E23" s="19">
-        <v>5000</v>
-      </c>
-      <c r="F23" s="19">
-        <v>0</v>
-      </c>
-      <c r="G23" s="19">
-        <v>5</v>
-      </c>
-      <c r="H23" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I23" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J23" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="K23" s="20">
-        <v>5</v>
-      </c>
-      <c r="L23" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="M23" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="71"/>
+      <c r="O23" s="71"/>
+      <c r="P23" s="71"/>
+      <c r="Q23" s="71"/>
+      <c r="R23" s="71"/>
+      <c r="S23" s="71"/>
+      <c r="T23" s="71"/>
+      <c r="U23" s="71"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B24" s="25">
         <v>50</v>
       </c>
-      <c r="C24" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="26">
-        <v>1000</v>
-      </c>
-      <c r="F24" s="26">
-        <v>0</v>
-      </c>
-      <c r="G24" s="26">
-        <v>5</v>
-      </c>
-      <c r="H24" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="I24" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J24" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="K24" s="28">
-        <v>10</v>
-      </c>
-      <c r="L24" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="M24" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="71"/>
+      <c r="O24" s="71"/>
+      <c r="P24" s="71"/>
+      <c r="Q24" s="71"/>
+      <c r="R24" s="71"/>
+      <c r="S24" s="71"/>
+      <c r="T24" s="71"/>
+      <c r="U24" s="71"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B25" s="26">
         <v>50</v>
       </c>
-      <c r="C25" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="26">
-        <v>750</v>
-      </c>
-      <c r="F25" s="26">
-        <v>0</v>
-      </c>
-      <c r="G25" s="26">
-        <v>5</v>
-      </c>
-      <c r="H25" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="I25" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="K25" s="28">
-        <v>10</v>
-      </c>
-      <c r="L25" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="M25" s="37" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="71"/>
+      <c r="O25" s="71"/>
+      <c r="P25" s="71"/>
+      <c r="Q25" s="71"/>
+      <c r="R25" s="71"/>
+      <c r="S25" s="71"/>
+      <c r="T25" s="71"/>
+      <c r="U25" s="71"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="B26" s="26">
         <v>50</v>
       </c>
-      <c r="C26" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="26">
-        <v>1500</v>
-      </c>
-      <c r="F26" s="26">
-        <v>0</v>
-      </c>
-      <c r="G26" s="26">
-        <v>5</v>
-      </c>
-      <c r="H26" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="I26" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J26" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="K26" s="28">
-        <v>10</v>
-      </c>
-      <c r="L26" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="M26" s="37" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="71"/>
+      <c r="O26" s="71"/>
+      <c r="P26" s="71"/>
+      <c r="Q26" s="71"/>
+      <c r="R26" s="71"/>
+      <c r="S26" s="71"/>
+      <c r="T26" s="71"/>
+      <c r="U26" s="71"/>
+    </row>
+    <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B27" s="19">
         <v>50</v>
       </c>
-      <c r="C27" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="E27" s="19">
-        <v>1000</v>
-      </c>
-      <c r="F27" s="19">
-        <v>0</v>
-      </c>
-      <c r="G27" s="19">
-        <v>5</v>
-      </c>
-      <c r="H27" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I27" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J27" s="19">
-        <v>32</v>
-      </c>
-      <c r="K27" s="20">
-        <v>10</v>
-      </c>
-      <c r="L27" s="42" t="s">
-        <v>153</v>
-      </c>
-      <c r="M27" s="37" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="42"/>
+      <c r="M27" s="37"/>
+      <c r="Q27" s="71"/>
+      <c r="R27" s="71"/>
+      <c r="S27" s="71"/>
+      <c r="T27" s="71"/>
+      <c r="U27" s="71"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q28" s="71"/>
+      <c r="R28" s="71"/>
+      <c r="S28" s="71"/>
+      <c r="T28" s="71"/>
+      <c r="U28" s="71"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q29" s="71"/>
+      <c r="R29" s="71"/>
+      <c r="S29" s="71"/>
+      <c r="T29" s="71"/>
+      <c r="U29" s="71"/>
+    </row>
+    <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q30" s="71"/>
+      <c r="R30" s="71"/>
+      <c r="S30" s="71"/>
+      <c r="T30" s="71"/>
+      <c r="U30" s="71"/>
+    </row>
+    <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>3</v>
@@ -2375,206 +2128,121 @@
         <v>7</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="K31" s="32" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="L31" s="24" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="M31" s="36" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="Q31" s="71"/>
+      <c r="R31" s="71"/>
+      <c r="S31" s="71"/>
+      <c r="T31" s="71"/>
+      <c r="U31" s="71"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="B32" s="18">
         <v>25</v>
       </c>
-      <c r="C32" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" s="19">
-        <v>500</v>
-      </c>
-      <c r="F32" s="19">
-        <v>0</v>
-      </c>
-      <c r="G32" s="19">
-        <v>5</v>
-      </c>
-      <c r="I32" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J32" s="15">
-        <v>64</v>
-      </c>
-      <c r="K32" s="20">
-        <v>10</v>
-      </c>
-      <c r="L32" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="M32" s="37" t="s">
-        <v>122</v>
-      </c>
+      <c r="C32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="37"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="B33" s="18">
         <v>25</v>
       </c>
-      <c r="C33" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="19">
-        <v>200</v>
-      </c>
-      <c r="F33" s="19">
-        <v>0</v>
-      </c>
-      <c r="G33" s="19">
-        <v>5</v>
-      </c>
-      <c r="I33" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J33" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="K33" s="20">
-        <v>10</v>
-      </c>
-      <c r="L33" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="M33" s="37" t="s">
-        <v>122</v>
-      </c>
+      <c r="C33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="37"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="B34" s="26">
         <v>25</v>
       </c>
-      <c r="C34" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="E34" s="26">
-        <v>1000</v>
-      </c>
-      <c r="F34" s="26">
-        <v>0</v>
-      </c>
-      <c r="G34" s="26">
-        <v>5</v>
-      </c>
-      <c r="I34" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="J34" s="26">
-        <v>16</v>
-      </c>
-      <c r="K34" s="28">
-        <v>10</v>
-      </c>
-      <c r="L34" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="M34" s="37" t="s">
-        <v>124</v>
-      </c>
+      <c r="C34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="37"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="B35" s="18">
         <v>50</v>
       </c>
-      <c r="C35" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="19">
-        <v>1250</v>
-      </c>
-      <c r="F35" s="18">
-        <v>0</v>
-      </c>
-      <c r="G35" s="18">
-        <v>5</v>
-      </c>
-      <c r="I35" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J35" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="K35" s="43">
-        <v>10</v>
-      </c>
-      <c r="L35" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="M35" s="37" t="s">
-        <v>124</v>
-      </c>
+      <c r="C35" s="18"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="37"/>
     </row>
     <row r="36" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="B36" s="18">
         <v>50</v>
       </c>
-      <c r="C36" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="E36" s="19">
-        <v>1250</v>
-      </c>
-      <c r="F36" s="18">
-        <v>0</v>
-      </c>
-      <c r="G36" s="18">
-        <v>5</v>
-      </c>
-      <c r="I36" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J36" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="K36" s="43">
-        <v>10</v>
-      </c>
-      <c r="L36" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="M36" s="37" t="s">
-        <v>124</v>
-      </c>
+      <c r="C36" s="18"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="42"/>
+      <c r="M36" s="37"/>
     </row>
     <row r="38" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="30" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>173</v>
+        <v>126</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>172</v>
+        <v>125</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>3</v>
@@ -2586,125 +2254,81 @@
         <v>5</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="I39" s="45" t="s">
         <v>7</v>
       </c>
       <c r="J39" s="47" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="K39" s="31" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="L39" s="44" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="M39" s="45" t="s">
-        <v>121</v>
-      </c>
-      <c r="O39" s="49" t="s">
-        <v>177</v>
-      </c>
-      <c r="P39" s="49"/>
-      <c r="Q39" s="49"/>
-      <c r="R39" s="49"/>
+        <v>90</v>
+      </c>
+      <c r="O39" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="51"/>
+      <c r="R39" s="51"/>
     </row>
     <row r="40" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="B40" s="14">
         <v>50</v>
       </c>
-      <c r="C40" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E40" s="14">
-        <v>1020</v>
-      </c>
-      <c r="F40" s="14">
-        <v>0</v>
-      </c>
-      <c r="G40" s="14">
-        <v>5</v>
-      </c>
-      <c r="H40" s="48" t="s">
-        <v>178</v>
-      </c>
-      <c r="I40" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J40" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="K40" s="14">
-        <v>10</v>
-      </c>
-      <c r="L40" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="O40" s="49"/>
-      <c r="P40" s="49"/>
-      <c r="Q40" s="49"/>
-      <c r="R40" s="49"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="48"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="5"/>
+      <c r="O40" s="51"/>
+      <c r="P40" s="51"/>
+      <c r="Q40" s="51"/>
+      <c r="R40" s="51"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="B41" s="14">
         <v>50</v>
       </c>
-      <c r="C41" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E41" s="14">
-        <v>1500</v>
-      </c>
-      <c r="F41" s="14">
-        <v>0</v>
-      </c>
-      <c r="G41" s="14">
-        <v>5</v>
-      </c>
-      <c r="H41" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="I41" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J41" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="K41" s="14">
-        <v>10</v>
-      </c>
-      <c r="L41" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="O41" s="49"/>
-      <c r="P41" s="49"/>
-      <c r="Q41" s="49"/>
-      <c r="R41" s="49"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="48"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="5"/>
+      <c r="O41" s="51"/>
+      <c r="P41" s="51"/>
+      <c r="Q41" s="51"/>
+      <c r="R41" s="51"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="49"/>
+      <c r="O42" s="51"/>
+      <c r="P42" s="51"/>
+      <c r="Q42" s="51"/>
+      <c r="R42" s="51"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="17"/>
@@ -2783,7 +2407,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2801,99 +2425,99 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+        <v>58</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+        <v>80</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+        <v>32</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="55"/>
+        <v>22</v>
+      </c>
+      <c r="B4" s="55" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="57"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="55"/>
+        <v>33</v>
+      </c>
+      <c r="B5" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="57"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
+        <v>92</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>128</v>
-      </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
+        <v>93</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>171</v>
-      </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
+        <v>123</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -2913,14 +2537,14 @@
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="E11" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="52"/>
+        <v>15</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>150</v>
+      </c>
+      <c r="G11" s="58"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="54"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="O11" s="10"/>
@@ -2929,16 +2553,16 @@
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>2</v>
@@ -2959,16 +2583,16 @@
         <v>7</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="L12" s="32" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="N12" s="33" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="O12" s="21"/>
       <c r="P12" s="10"/>
@@ -2976,19 +2600,19 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C13" s="14">
         <v>25</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="14">
         <v>50</v>
@@ -3012,10 +2636,10 @@
         <v>5</v>
       </c>
       <c r="M13" s="14" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="N13" s="14" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="O13" s="21"/>
       <c r="P13" s="10"/>
@@ -3023,19 +2647,19 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C14" s="19">
         <v>25</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="19">
         <v>50</v>
@@ -3053,16 +2677,16 @@
         <v>9</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="L14" s="20">
         <v>5</v>
       </c>
       <c r="M14" s="19" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="O14" s="21"/>
       <c r="P14" s="10"/>
@@ -3070,19 +2694,19 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C15" s="19">
         <v>25</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F15" s="19">
         <v>50</v>
@@ -3100,33 +2724,33 @@
         <v>9</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="L15" s="20">
         <v>5</v>
       </c>
       <c r="M15" s="19" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C16" s="26">
         <v>25</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F16" s="26">
         <v>100</v>
@@ -3138,39 +2762,39 @@
         <v>5</v>
       </c>
       <c r="I16" s="26" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="J16" s="26" t="s">
         <v>9</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L16" s="28">
         <v>5</v>
       </c>
       <c r="M16" s="26" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="N16" s="26" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C17" s="19">
         <v>20</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" s="19">
         <v>500</v>
@@ -3188,16 +2812,16 @@
         <v>9</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="L17" s="19">
         <v>5</v>
       </c>
       <c r="M17" s="19" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="N17" s="19" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="O17" s="21"/>
       <c r="P17" s="10"/>
@@ -3205,19 +2829,19 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C18" s="19">
         <v>20</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F18" s="19">
         <v>640</v>
@@ -3235,19 +2859,19 @@
         <v>9</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="L18" s="19">
         <v>5</v>
       </c>
       <c r="M18" s="19" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>145</v>
+        <v>103</v>
       </c>
       <c r="O18" s="21" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
@@ -3259,19 +2883,19 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C20" s="19">
         <v>25</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F20" s="19">
         <v>110</v>
@@ -3289,16 +2913,16 @@
         <v>9</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="L20" s="19">
         <v>5</v>
       </c>
       <c r="M20" s="19" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="O20" s="21"/>
       <c r="P20" s="10"/>
@@ -3306,19 +2930,19 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C21" s="19">
         <v>25</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F21" s="19">
         <v>500</v>
@@ -3342,28 +2966,28 @@
         <v>5</v>
       </c>
       <c r="M21" s="19" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="N21" s="19" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="O21" s="17"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C22" s="19">
         <v>25</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="F22" s="19">
         <v>1000</v>
@@ -3375,7 +2999,7 @@
         <v>5</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="J22" s="19" t="s">
         <v>9</v>
@@ -3387,27 +3011,27 @@
         <v>5</v>
       </c>
       <c r="M22" s="19" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="N22" s="19" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C23" s="19">
         <v>25</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23" s="19">
         <v>500</v>
@@ -3419,37 +3043,37 @@
         <v>5</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>156</v>
+        <v>112</v>
       </c>
       <c r="J23" s="19" t="s">
         <v>9</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="L23" s="19">
         <v>5</v>
       </c>
       <c r="M23" s="19" t="s">
-        <v>157</v>
+        <v>113</v>
       </c>
       <c r="N23" s="19" t="s">
-        <v>158</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>3</v>
@@ -3464,30 +3088,30 @@
         <v>7</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="L26" s="32" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="M26" s="12" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="N26" s="33" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C27" s="14">
         <v>10</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="F27" s="14">
         <v>100</v>
@@ -3508,24 +3132,24 @@
         <v>5</v>
       </c>
       <c r="M27" s="14" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="N27" s="14" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C28" s="14">
         <v>20</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="F28" s="14">
         <v>500</v>
@@ -3540,30 +3164,30 @@
         <v>9</v>
       </c>
       <c r="K28" s="15" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="L28" s="15">
         <v>5</v>
       </c>
       <c r="M28" s="14" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="N28" s="14" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C29" s="14">
         <v>20</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="F29" s="14">
         <v>500</v>
@@ -3584,28 +3208,28 @@
         <v>5</v>
       </c>
       <c r="M29" s="14" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="N29" s="14" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D32" s="46" t="s">
-        <v>173</v>
-      </c>
-      <c r="E32" s="61" t="s">
-        <v>172</v>
+        <v>126</v>
+      </c>
+      <c r="E32" s="50" t="s">
+        <v>125</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>3</v>
@@ -3620,33 +3244,33 @@
         <v>7</v>
       </c>
       <c r="K32" s="7" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="L32" s="32" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="M32" s="12" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="N32" s="33" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C33" s="14">
         <v>20</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="F33" s="14">
         <v>510</v>
@@ -3661,33 +3285,33 @@
         <v>9</v>
       </c>
       <c r="K33" s="15" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L33" s="15">
         <v>5</v>
       </c>
       <c r="M33" s="14" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="N33" s="14" t="s">
-        <v>187</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C34" s="14">
         <v>20</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="F34" s="14">
         <v>530</v>
@@ -3702,29 +3326,29 @@
         <v>9</v>
       </c>
       <c r="K34" s="15" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="L34" s="15">
         <v>5</v>
       </c>
       <c r="M34" s="14" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="N34" s="14" t="s">
-        <v>188</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="F11:I11"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="F11:I11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3735,7 +3359,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3754,79 +3378,79 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+        <v>58</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+        <v>80</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+        <v>32</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="O4" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
+        <v>92</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="O4" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="57"/>
-      <c r="Q5" s="57"/>
-      <c r="R5" s="57"/>
+        <v>93</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O6" s="57"/>
-      <c r="P6" s="57"/>
-      <c r="Q6" s="57"/>
-      <c r="R6" s="57"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="60"/>
+      <c r="Q6" s="60"/>
+      <c r="R6" s="60"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
@@ -3835,33 +3459,33 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="E7" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="G7" s="52"/>
+        <v>16</v>
+      </c>
+      <c r="F7" s="53" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" s="54"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
-      <c r="O7" s="57"/>
-      <c r="P7" s="57"/>
-      <c r="Q7" s="57"/>
-      <c r="R7" s="57"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="60"/>
+      <c r="Q7" s="60"/>
+      <c r="R7" s="60"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>2</v>
@@ -3882,30 +3506,30 @@
         <v>7</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="M8" s="35" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C9" s="14">
         <v>25</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="14">
         <v>180</v>
@@ -3926,27 +3550,27 @@
         <v>16</v>
       </c>
       <c r="L9" s="14" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C10" s="19">
         <v>20</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="19">
         <v>100</v>
@@ -3967,34 +3591,34 @@
         <v>16</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="M10" s="19" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="N10" s="17"/>
-      <c r="O10" s="59" t="s">
-        <v>147</v>
-      </c>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="59"/>
-      <c r="R10" s="59"/>
+      <c r="O10" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="62"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C11" s="19">
         <v>20</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" s="19">
         <v>200</v>
@@ -4015,32 +3639,32 @@
         <v>16</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="M11" s="19" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="N11" s="17"/>
-      <c r="O11" s="59"/>
-      <c r="P11" s="59"/>
-      <c r="Q11" s="59"/>
-      <c r="R11" s="59"/>
+      <c r="O11" s="62"/>
+      <c r="P11" s="62"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="62"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C12" s="19">
         <v>20</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F12" s="19">
         <v>200</v>
@@ -4061,32 +3685,32 @@
         <v>16</v>
       </c>
       <c r="L12" s="19" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="M12" s="19" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="N12" s="17"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="59"/>
-      <c r="R12" s="59"/>
+      <c r="O12" s="62"/>
+      <c r="P12" s="62"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="62"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C13" s="19">
         <v>20</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="F13" s="19">
         <v>200</v>
@@ -4098,19 +3722,19 @@
         <v>5</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="J13" s="19" t="s">
         <v>9</v>
       </c>
       <c r="K13" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="M13" s="19" t="s">
         <v>50</v>
-      </c>
-      <c r="L13" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="M13" s="19" t="s">
-        <v>68</v>
       </c>
       <c r="N13" s="17"/>
       <c r="O13" s="17"/>
@@ -4119,19 +3743,19 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C14" s="14">
         <v>20</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F14" s="14">
         <v>500</v>
@@ -4152,20 +3776,20 @@
         <v>32</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="N14" s="41" t="s">
-        <v>135</v>
-      </c>
-      <c r="O14" s="56" t="s">
-        <v>136</v>
-      </c>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
-      <c r="R14" s="57"/>
+        <v>98</v>
+      </c>
+      <c r="O14" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="P14" s="60"/>
+      <c r="Q14" s="60"/>
+      <c r="R14" s="60"/>
     </row>
     <row r="15" spans="1:18" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
@@ -4182,26 +3806,26 @@
       <c r="L15" s="40"/>
       <c r="M15" s="40"/>
       <c r="N15" s="17"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="57"/>
-      <c r="R15" s="57"/>
+      <c r="O15" s="60"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="60"/>
+      <c r="R15" s="60"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C16" s="26">
         <v>20</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F16" s="26">
         <v>1000</v>
@@ -4222,32 +3846,32 @@
         <v>32</v>
       </c>
       <c r="L16" s="26" t="s">
-        <v>102</v>
+        <v>79</v>
       </c>
       <c r="M16" s="26" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="N16" s="17"/>
-      <c r="O16" s="57"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="57"/>
-      <c r="R16" s="57"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="60"/>
+      <c r="R16" s="60"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C17" s="19">
         <v>20</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" s="19">
         <v>450</v>
@@ -4265,35 +3889,35 @@
         <v>9</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="L17" s="19" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="M17" s="19" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="N17" s="17"/>
-      <c r="O17" s="57"/>
-      <c r="P17" s="57"/>
-      <c r="Q17" s="57"/>
-      <c r="R17" s="57"/>
+      <c r="O17" s="60"/>
+      <c r="P17" s="60"/>
+      <c r="Q17" s="60"/>
+      <c r="R17" s="60"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C18" s="26">
         <v>20</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F18" s="26">
         <v>1000</v>
@@ -4311,35 +3935,35 @@
         <v>9</v>
       </c>
       <c r="K18" s="26" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="L18" s="26" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="M18" s="26" t="s">
-        <v>150</v>
+        <v>108</v>
       </c>
       <c r="N18" s="17"/>
-      <c r="O18" s="57"/>
-      <c r="P18" s="57"/>
-      <c r="Q18" s="57"/>
-      <c r="R18" s="57"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="60"/>
+      <c r="R18" s="60"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C19" s="19">
         <v>20</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F19" s="19">
         <v>1000</v>
@@ -4357,35 +3981,35 @@
         <v>9</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>154</v>
+        <v>110</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
       <c r="M19" s="19" t="s">
-        <v>159</v>
+        <v>115</v>
       </c>
       <c r="N19" s="17"/>
-      <c r="O19" s="58"/>
-      <c r="P19" s="58"/>
-      <c r="Q19" s="58"/>
-      <c r="R19" s="58"/>
+      <c r="O19" s="61"/>
+      <c r="P19" s="61"/>
+      <c r="Q19" s="61"/>
+      <c r="R19" s="61"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C20" s="19">
         <v>20</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20" s="19">
         <v>1000</v>
@@ -4403,13 +4027,13 @@
         <v>9</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>160</v>
+        <v>116</v>
       </c>
       <c r="L20" s="19" t="s">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="M20" s="19" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
       <c r="N20" s="17"/>
       <c r="O20" s="17"/>
@@ -4437,16 +4061,16 @@
     </row>
     <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="34" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="3" t="s">
@@ -4462,13 +4086,13 @@
         <v>7</v>
       </c>
       <c r="K22" s="7" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="M22" s="35" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
@@ -4477,16 +4101,16 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C23" s="14">
         <v>20</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="F23" s="14">
         <v>850</v>
@@ -4501,13 +4125,13 @@
         <v>9</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>165</v>
+        <v>120</v>
       </c>
       <c r="M23" s="14" t="s">
-        <v>166</v>
+        <v>121</v>
       </c>
       <c r="N23" s="17"/>
       <c r="O23" s="17"/>
@@ -4567,24 +4191,24 @@
     </row>
     <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="34" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D27" s="46" t="s">
-        <v>173</v>
+        <v>126</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>172</v>
+        <v>125</v>
       </c>
       <c r="F27" s="47" t="s">
-        <v>182</v>
-      </c>
-      <c r="G27" s="60" t="s">
+        <v>132</v>
+      </c>
+      <c r="G27" s="49" t="s">
         <v>3</v>
       </c>
       <c r="H27" s="2" t="s">
@@ -4597,35 +4221,35 @@
         <v>7</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="L27" s="12" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="M27" s="35" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="O27" s="17"/>
       <c r="P27" s="17"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C28" s="14">
         <v>20</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="F28" s="48" t="s">
-        <v>179</v>
+        <v>130</v>
       </c>
       <c r="G28" s="14">
         <v>250</v>
@@ -4640,13 +4264,13 @@
         <v>9</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="L28" s="14" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="M28" s="48" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -4654,12 +4278,12 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>151</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -4683,8 +4307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4699,39 +4323,39 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+        <v>58</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+        <v>80</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+        <v>32</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -4740,27 +4364,27 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
+        <v>92</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
+        <v>93</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L8" s="22"/>
@@ -4772,12 +4396,12 @@
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="51" t="s">
-        <v>137</v>
-      </c>
-      <c r="F9" s="52"/>
+        <v>17</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="F9" s="54"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -4787,13 +4411,13 @@
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>2</v>
@@ -4814,197 +4438,87 @@
         <v>7</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B11" s="14">
-        <v>10</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="14">
-        <v>100</v>
-      </c>
-      <c r="F11" s="14">
-        <v>0</v>
-      </c>
-      <c r="G11" s="14">
-        <v>2</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="14">
-        <v>64</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>105</v>
-      </c>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="19">
-        <v>10</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12" s="19">
-        <v>400</v>
-      </c>
-      <c r="F12" s="19">
-        <v>0</v>
-      </c>
-      <c r="G12" s="19">
-        <v>2</v>
-      </c>
-      <c r="H12" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>106</v>
-      </c>
+      <c r="A12" s="14"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" s="19">
-        <v>20</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" s="19">
-        <v>160</v>
-      </c>
-      <c r="F13" s="19">
-        <v>0</v>
-      </c>
-      <c r="G13" s="19">
-        <v>5</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>118</v>
-      </c>
+      <c r="A13" s="14"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="B14" s="19">
-        <v>15</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" s="19">
-        <v>520</v>
-      </c>
-      <c r="F14" s="19">
-        <v>0</v>
-      </c>
-      <c r="G14" s="19">
-        <v>2</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="K14" s="19" t="s">
-        <v>164</v>
-      </c>
+      <c r="A14" s="14"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="B15" s="19">
-        <v>15</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" s="19">
-        <v>470</v>
-      </c>
-      <c r="F15" s="19">
-        <v>0</v>
-      </c>
-      <c r="G15" s="19">
-        <v>2</v>
-      </c>
-      <c r="H15" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="K15" s="19" t="s">
-        <v>168</v>
-      </c>
+      <c r="A15" s="14"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
@@ -5023,45 +4537,25 @@
         <v>7</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="L18" s="17"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B19" s="14">
-        <v>20</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>78</v>
-      </c>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="14"/>
-      <c r="E19" s="14">
-        <v>460</v>
-      </c>
-      <c r="F19" s="14">
-        <v>0</v>
-      </c>
-      <c r="G19" s="14">
-        <v>5</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="K19" s="14" t="s">
-        <v>119</v>
-      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
       <c r="L19" s="17"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
EVA settings changed + minor stuff
</commit_message>
<xml_diff>
--- a/Experiments/comparison.xlsx
+++ b/Experiments/comparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2048" sheetId="1" r:id="rId1"/>
@@ -529,9 +529,6 @@
     <t>Race config</t>
   </si>
   <si>
-    <t>1 lap, Alalborg, Score: distance_raced / lap_time</t>
-  </si>
-  <si>
     <t>esn: 1024, ro:256</t>
   </si>
   <si>
@@ -539,6 +536,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 17.59% (44/250)</t>
+  </si>
+  <si>
+    <t>1 lap, Aalborg, Score: distance_raced / lap_time</t>
   </si>
 </sst>
 </file>
@@ -1145,40 +1145,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1208,6 +1174,40 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -1518,7 +1518,7 @@
   <dimension ref="A1:U111"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,78 +1539,78 @@
       <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S8" s="67"/>
-      <c r="T8" s="67"/>
-      <c r="U8" s="67"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="55"/>
+      <c r="U8" s="55"/>
     </row>
     <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
@@ -1621,19 +1621,19 @@
       <c r="D9" s="11">
         <v>2048</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="F9" s="52"/>
+      <c r="F9" s="69"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="23"/>
       <c r="L9" s="8"/>
-      <c r="S9" s="67"/>
-      <c r="T9" s="67"/>
-      <c r="U9" s="67"/>
+      <c r="S9" s="55"/>
+      <c r="T9" s="55"/>
+      <c r="U9" s="55"/>
     </row>
     <row r="10" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1672,16 +1672,16 @@
       <c r="L10" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="N10" s="61" t="s">
+      <c r="N10" s="49" t="s">
         <v>139</v>
       </c>
-      <c r="O10" s="62"/>
-      <c r="P10" s="63"/>
-      <c r="Q10" s="63"/>
-      <c r="R10" s="73"/>
-      <c r="S10" s="67"/>
-      <c r="T10" s="67"/>
-      <c r="U10" s="67"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="61"/>
+      <c r="S10" s="55"/>
+      <c r="T10" s="55"/>
+      <c r="U10" s="55"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
@@ -1720,14 +1720,14 @@
       <c r="L11" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="N11" s="64"/>
-      <c r="O11" s="65"/>
-      <c r="P11" s="66"/>
-      <c r="Q11" s="66"/>
-      <c r="R11" s="74"/>
-      <c r="S11" s="67"/>
-      <c r="T11" s="67"/>
-      <c r="U11" s="67"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="53"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="62"/>
+      <c r="S11" s="55"/>
+      <c r="T11" s="55"/>
+      <c r="U11" s="55"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
@@ -1766,16 +1766,16 @@
       <c r="L12" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="N12" s="64" t="s">
+      <c r="N12" s="52" t="s">
         <v>140</v>
       </c>
-      <c r="O12" s="65"/>
-      <c r="P12" s="66"/>
-      <c r="Q12" s="66"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="67"/>
-      <c r="T12" s="67"/>
-      <c r="U12" s="67"/>
+      <c r="O12" s="53"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="62"/>
+      <c r="S12" s="55"/>
+      <c r="T12" s="55"/>
+      <c r="U12" s="55"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
@@ -1814,16 +1814,16 @@
       <c r="L13" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="N13" s="64" t="s">
+      <c r="N13" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="O13" s="65"/>
-      <c r="P13" s="66"/>
-      <c r="Q13" s="66"/>
-      <c r="R13" s="74"/>
-      <c r="S13" s="67"/>
-      <c r="T13" s="67"/>
-      <c r="U13" s="67"/>
+      <c r="O13" s="53"/>
+      <c r="P13" s="54"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="55"/>
+      <c r="T13" s="55"/>
+      <c r="U13" s="55"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
@@ -1862,16 +1862,16 @@
       <c r="L14" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="N14" s="75" t="s">
+      <c r="N14" s="63" t="s">
         <v>154</v>
       </c>
-      <c r="O14" s="65"/>
-      <c r="P14" s="66"/>
-      <c r="Q14" s="66"/>
-      <c r="R14" s="74"/>
-      <c r="S14" s="67"/>
-      <c r="T14" s="67"/>
-      <c r="U14" s="67"/>
+      <c r="O14" s="53"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="55"/>
+      <c r="T14" s="55"/>
+      <c r="U14" s="55"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
@@ -1910,14 +1910,14 @@
       <c r="L15" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="N15" s="64"/>
-      <c r="O15" s="65"/>
-      <c r="P15" s="66"/>
-      <c r="Q15" s="66"/>
-      <c r="R15" s="74"/>
-      <c r="S15" s="67"/>
-      <c r="T15" s="67"/>
-      <c r="U15" s="67"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="54"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="55"/>
+      <c r="T15" s="55"/>
+      <c r="U15" s="55"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
@@ -1936,16 +1936,16 @@
       <c r="J16" s="15"/>
       <c r="K16" s="20"/>
       <c r="L16" s="16"/>
-      <c r="N16" s="64" t="s">
+      <c r="N16" s="52" t="s">
         <v>141</v>
       </c>
-      <c r="O16" s="65"/>
-      <c r="P16" s="66"/>
-      <c r="Q16" s="66"/>
-      <c r="R16" s="74"/>
-      <c r="S16" s="67"/>
-      <c r="T16" s="67"/>
-      <c r="U16" s="67"/>
+      <c r="O16" s="53"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="62"/>
+      <c r="S16" s="55"/>
+      <c r="T16" s="55"/>
+      <c r="U16" s="55"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
@@ -1964,16 +1964,16 @@
       <c r="J17" s="20"/>
       <c r="K17" s="20"/>
       <c r="L17" s="16"/>
-      <c r="N17" s="64" t="s">
+      <c r="N17" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="O17" s="65"/>
-      <c r="P17" s="66"/>
-      <c r="Q17" s="66"/>
-      <c r="R17" s="74"/>
-      <c r="S17" s="67"/>
-      <c r="T17" s="67"/>
-      <c r="U17" s="67"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="55"/>
+      <c r="T17" s="55"/>
+      <c r="U17" s="55"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
@@ -1992,16 +1992,16 @@
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
       <c r="L18" s="16"/>
-      <c r="N18" s="64" t="s">
+      <c r="N18" s="52" t="s">
         <v>143</v>
       </c>
-      <c r="O18" s="65"/>
-      <c r="P18" s="66"/>
-      <c r="Q18" s="66"/>
-      <c r="R18" s="74"/>
-      <c r="S18" s="67"/>
-      <c r="T18" s="67"/>
-      <c r="U18" s="67"/>
+      <c r="O18" s="53"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="62"/>
+      <c r="S18" s="55"/>
+      <c r="T18" s="55"/>
+      <c r="U18" s="55"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
@@ -2020,16 +2020,16 @@
       <c r="J19" s="20"/>
       <c r="K19" s="20"/>
       <c r="L19" s="16"/>
-      <c r="N19" s="64" t="s">
+      <c r="N19" s="52" t="s">
         <v>144</v>
       </c>
-      <c r="O19" s="65"/>
-      <c r="P19" s="66"/>
-      <c r="Q19" s="66"/>
-      <c r="R19" s="74"/>
-      <c r="S19" s="67"/>
-      <c r="T19" s="67"/>
-      <c r="U19" s="67"/>
+      <c r="O19" s="53"/>
+      <c r="P19" s="54"/>
+      <c r="Q19" s="54"/>
+      <c r="R19" s="62"/>
+      <c r="S19" s="55"/>
+      <c r="T19" s="55"/>
+      <c r="U19" s="55"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
@@ -2048,16 +2048,16 @@
       <c r="J20" s="15"/>
       <c r="K20" s="20"/>
       <c r="L20" s="16"/>
-      <c r="N20" s="64" t="s">
+      <c r="N20" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="O20" s="65"/>
-      <c r="P20" s="66"/>
-      <c r="Q20" s="66"/>
-      <c r="R20" s="74"/>
-      <c r="S20" s="67"/>
-      <c r="T20" s="67"/>
-      <c r="U20" s="67"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="62"/>
+      <c r="S20" s="55"/>
+      <c r="T20" s="55"/>
+      <c r="U20" s="55"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
@@ -2076,16 +2076,16 @@
       <c r="J21" s="15"/>
       <c r="K21" s="20"/>
       <c r="L21" s="16"/>
-      <c r="N21" s="68" t="s">
+      <c r="N21" s="56" t="s">
         <v>146</v>
       </c>
-      <c r="O21" s="69"/>
-      <c r="P21" s="66"/>
-      <c r="Q21" s="66"/>
-      <c r="R21" s="74"/>
-      <c r="S21" s="67"/>
-      <c r="T21" s="67"/>
-      <c r="U21" s="67"/>
+      <c r="O21" s="57"/>
+      <c r="P21" s="54"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="62"/>
+      <c r="S21" s="55"/>
+      <c r="T21" s="55"/>
+      <c r="U21" s="55"/>
     </row>
     <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
@@ -2104,16 +2104,16 @@
       <c r="J22" s="15"/>
       <c r="K22" s="20"/>
       <c r="L22" s="16"/>
-      <c r="N22" s="70" t="s">
+      <c r="N22" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="O22" s="71"/>
-      <c r="P22" s="72"/>
-      <c r="Q22" s="72"/>
-      <c r="R22" s="76"/>
-      <c r="S22" s="67"/>
-      <c r="T22" s="67"/>
-      <c r="U22" s="67"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="60"/>
+      <c r="Q22" s="60"/>
+      <c r="R22" s="64"/>
+      <c r="S22" s="55"/>
+      <c r="T22" s="55"/>
+      <c r="U22" s="55"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
@@ -2132,14 +2132,14 @@
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
       <c r="L23" s="16"/>
-      <c r="N23" s="67"/>
-      <c r="O23" s="67"/>
-      <c r="P23" s="67"/>
-      <c r="Q23" s="67"/>
-      <c r="R23" s="67"/>
-      <c r="S23" s="67"/>
-      <c r="T23" s="67"/>
-      <c r="U23" s="67"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="55"/>
+      <c r="P23" s="55"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="55"/>
+      <c r="S23" s="55"/>
+      <c r="T23" s="55"/>
+      <c r="U23" s="55"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
@@ -2158,14 +2158,14 @@
       <c r="J24" s="28"/>
       <c r="K24" s="28"/>
       <c r="L24" s="36"/>
-      <c r="N24" s="67"/>
-      <c r="O24" s="67"/>
-      <c r="P24" s="67"/>
-      <c r="Q24" s="67"/>
-      <c r="R24" s="67"/>
-      <c r="S24" s="67"/>
-      <c r="T24" s="67"/>
-      <c r="U24" s="67"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="55"/>
+      <c r="P24" s="55"/>
+      <c r="Q24" s="55"/>
+      <c r="R24" s="55"/>
+      <c r="S24" s="55"/>
+      <c r="T24" s="55"/>
+      <c r="U24" s="55"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
@@ -2184,13 +2184,13 @@
       <c r="J25" s="26"/>
       <c r="K25" s="28"/>
       <c r="L25" s="36"/>
-      <c r="N25" s="67"/>
-      <c r="O25" s="67"/>
-      <c r="P25" s="67"/>
-      <c r="Q25" s="67"/>
-      <c r="R25" s="67"/>
-      <c r="S25" s="67"/>
-      <c r="U25" s="67"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="55"/>
+      <c r="P25" s="55"/>
+      <c r="Q25" s="55"/>
+      <c r="R25" s="55"/>
+      <c r="S25" s="55"/>
+      <c r="U25" s="55"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
@@ -2209,14 +2209,14 @@
       <c r="J26" s="26"/>
       <c r="K26" s="28"/>
       <c r="L26" s="37"/>
-      <c r="N26" s="67"/>
-      <c r="O26" s="67"/>
-      <c r="P26" s="67"/>
-      <c r="Q26" s="67"/>
-      <c r="R26" s="67"/>
-      <c r="S26" s="67"/>
-      <c r="T26" s="67"/>
-      <c r="U26" s="67"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
+      <c r="P26" s="55"/>
+      <c r="Q26" s="55"/>
+      <c r="R26" s="55"/>
+      <c r="S26" s="55"/>
+      <c r="T26" s="55"/>
+      <c r="U26" s="55"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="19" t="s">
@@ -2235,32 +2235,32 @@
       <c r="J27" s="19"/>
       <c r="K27" s="20"/>
       <c r="L27" s="40"/>
-      <c r="Q27" s="67"/>
-      <c r="R27" s="67"/>
-      <c r="S27" s="67"/>
-      <c r="T27" s="67"/>
-      <c r="U27" s="67"/>
+      <c r="Q27" s="55"/>
+      <c r="R27" s="55"/>
+      <c r="S27" s="55"/>
+      <c r="T27" s="55"/>
+      <c r="U27" s="55"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="Q28" s="67"/>
-      <c r="R28" s="67"/>
-      <c r="S28" s="67"/>
-      <c r="T28" s="67"/>
-      <c r="U28" s="67"/>
+      <c r="Q28" s="55"/>
+      <c r="R28" s="55"/>
+      <c r="S28" s="55"/>
+      <c r="T28" s="55"/>
+      <c r="U28" s="55"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="Q29" s="67"/>
-      <c r="R29" s="67"/>
-      <c r="S29" s="67"/>
-      <c r="T29" s="67"/>
-      <c r="U29" s="67"/>
+      <c r="Q29" s="55"/>
+      <c r="R29" s="55"/>
+      <c r="S29" s="55"/>
+      <c r="T29" s="55"/>
+      <c r="U29" s="55"/>
     </row>
     <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q30" s="67"/>
-      <c r="R30" s="67"/>
-      <c r="S30" s="67"/>
-      <c r="T30" s="67"/>
-      <c r="U30" s="67"/>
+      <c r="Q30" s="55"/>
+      <c r="R30" s="55"/>
+      <c r="S30" s="55"/>
+      <c r="T30" s="55"/>
+      <c r="U30" s="55"/>
     </row>
     <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
@@ -2293,11 +2293,11 @@
       <c r="L31" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="Q31" s="67"/>
-      <c r="R31" s="67"/>
-      <c r="S31" s="67"/>
-      <c r="T31" s="67"/>
-      <c r="U31" s="67"/>
+      <c r="Q31" s="55"/>
+      <c r="R31" s="55"/>
+      <c r="S31" s="55"/>
+      <c r="T31" s="55"/>
+      <c r="U31" s="55"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
@@ -2417,12 +2417,12 @@
       <c r="L39" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="O39" s="49" t="s">
+      <c r="O39" s="66" t="s">
         <v>129</v>
       </c>
-      <c r="P39" s="49"/>
-      <c r="Q39" s="49"/>
-      <c r="R39" s="49"/>
+      <c r="P39" s="66"/>
+      <c r="Q39" s="66"/>
+      <c r="R39" s="66"/>
     </row>
     <row r="40" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
@@ -2441,10 +2441,10 @@
       <c r="J40" s="14"/>
       <c r="K40" s="14"/>
       <c r="L40" s="14"/>
-      <c r="O40" s="49"/>
-      <c r="P40" s="49"/>
-      <c r="Q40" s="49"/>
-      <c r="R40" s="49"/>
+      <c r="O40" s="66"/>
+      <c r="P40" s="66"/>
+      <c r="Q40" s="66"/>
+      <c r="R40" s="66"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
@@ -2463,16 +2463,16 @@
       <c r="J41" s="14"/>
       <c r="K41" s="14"/>
       <c r="L41" s="14"/>
-      <c r="O41" s="49"/>
-      <c r="P41" s="49"/>
-      <c r="Q41" s="49"/>
-      <c r="R41" s="49"/>
+      <c r="O41" s="66"/>
+      <c r="P41" s="66"/>
+      <c r="Q41" s="66"/>
+      <c r="R41" s="66"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="49"/>
+      <c r="O42" s="66"/>
+      <c r="P42" s="66"/>
+      <c r="Q42" s="66"/>
+      <c r="R42" s="66"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="17"/>
@@ -2549,8 +2549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2570,97 +2570,97 @@
       <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="55"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="73"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="55"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="73"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -2682,12 +2682,12 @@
       <c r="E11" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="52"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="69"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="O11" s="10"/>
@@ -3288,10 +3288,10 @@
         <v>5</v>
       </c>
       <c r="M26" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="N26" s="19" t="s">
         <v>172</v>
-      </c>
-      <c r="N26" s="19" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3613,77 +3613,77 @@
       <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="O4" s="58" t="s">
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="O4" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="58"/>
+      <c r="P4" s="75"/>
+      <c r="Q4" s="75"/>
+      <c r="R4" s="75"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="58"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="75"/>
+      <c r="R5" s="75"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
+      <c r="O6" s="75"/>
+      <c r="P6" s="75"/>
+      <c r="Q6" s="75"/>
+      <c r="R6" s="75"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
@@ -3694,18 +3694,18 @@
       <c r="E7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="68" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="52"/>
+      <c r="G7" s="69"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="58"/>
-      <c r="R7" s="58"/>
+      <c r="O7" s="75"/>
+      <c r="P7" s="75"/>
+      <c r="Q7" s="75"/>
+      <c r="R7" s="75"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
@@ -3830,12 +3830,12 @@
         <v>43</v>
       </c>
       <c r="N10" s="17"/>
-      <c r="O10" s="60" t="s">
+      <c r="O10" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
+      <c r="P10" s="77"/>
+      <c r="Q10" s="77"/>
+      <c r="R10" s="77"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
@@ -3878,10 +3878,10 @@
         <v>46</v>
       </c>
       <c r="N11" s="17"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="60"/>
+      <c r="O11" s="77"/>
+      <c r="P11" s="77"/>
+      <c r="Q11" s="77"/>
+      <c r="R11" s="77"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
@@ -3924,10 +3924,10 @@
         <v>48</v>
       </c>
       <c r="N12" s="17"/>
-      <c r="O12" s="60"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="60"/>
-      <c r="R12" s="60"/>
+      <c r="O12" s="77"/>
+      <c r="P12" s="77"/>
+      <c r="Q12" s="77"/>
+      <c r="R12" s="77"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
@@ -4017,12 +4017,12 @@
       <c r="N14" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="O14" s="57" t="s">
+      <c r="O14" s="74" t="s">
         <v>99</v>
       </c>
-      <c r="P14" s="58"/>
-      <c r="Q14" s="58"/>
-      <c r="R14" s="58"/>
+      <c r="P14" s="75"/>
+      <c r="Q14" s="75"/>
+      <c r="R14" s="75"/>
     </row>
     <row r="15" spans="1:18" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38"/>
@@ -4039,10 +4039,10 @@
       <c r="L15" s="38"/>
       <c r="M15" s="38"/>
       <c r="N15" s="17"/>
-      <c r="O15" s="58"/>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="58"/>
-      <c r="R15" s="58"/>
+      <c r="O15" s="75"/>
+      <c r="P15" s="75"/>
+      <c r="Q15" s="75"/>
+      <c r="R15" s="75"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
@@ -4085,10 +4085,10 @@
         <v>106</v>
       </c>
       <c r="N16" s="17"/>
-      <c r="O16" s="58"/>
-      <c r="P16" s="58"/>
-      <c r="Q16" s="58"/>
-      <c r="R16" s="58"/>
+      <c r="O16" s="75"/>
+      <c r="P16" s="75"/>
+      <c r="Q16" s="75"/>
+      <c r="R16" s="75"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
@@ -4131,10 +4131,10 @@
         <v>107</v>
       </c>
       <c r="N17" s="17"/>
-      <c r="O17" s="58"/>
-      <c r="P17" s="58"/>
-      <c r="Q17" s="58"/>
-      <c r="R17" s="58"/>
+      <c r="O17" s="75"/>
+      <c r="P17" s="75"/>
+      <c r="Q17" s="75"/>
+      <c r="R17" s="75"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -4177,10 +4177,10 @@
         <v>108</v>
       </c>
       <c r="N18" s="17"/>
-      <c r="O18" s="58"/>
-      <c r="P18" s="58"/>
-      <c r="Q18" s="58"/>
-      <c r="R18" s="58"/>
+      <c r="O18" s="75"/>
+      <c r="P18" s="75"/>
+      <c r="Q18" s="75"/>
+      <c r="R18" s="75"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
@@ -4223,10 +4223,10 @@
         <v>115</v>
       </c>
       <c r="N19" s="17"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="59"/>
-      <c r="R19" s="59"/>
+      <c r="O19" s="76"/>
+      <c r="P19" s="76"/>
+      <c r="Q19" s="76"/>
+      <c r="R19" s="76"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
@@ -4540,8 +4540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4560,37 +4560,37 @@
       <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -4601,25 +4601,25 @@
       <c r="A4" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L8" s="22"/>
@@ -4633,10 +4633,10 @@
       <c r="D9" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="68" t="s">
         <v>150</v>
       </c>
-      <c r="F9" s="52"/>
+      <c r="F9" s="69"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -4711,13 +4711,13 @@
         <v>9</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K11" s="15" t="s">
         <v>168</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -4732,7 +4732,7 @@
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="20"/>
-      <c r="L12" s="77"/>
+      <c r="L12" s="65"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -4746,7 +4746,7 @@
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
       <c r="K13" s="20"/>
-      <c r="L13" s="77"/>
+      <c r="L13" s="65"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
@@ -4760,7 +4760,7 @@
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
       <c r="K14" s="20"/>
-      <c r="L14" s="77"/>
+      <c r="L14" s="65"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
@@ -4774,7 +4774,7 @@
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
       <c r="K15" s="20"/>
-      <c r="L15" s="77"/>
+      <c r="L15" s="65"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Experiments + small changes
</commit_message>
<xml_diff>
--- a/Experiments/comparison.xlsx
+++ b/Experiments/comparison.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="185">
   <si>
     <t>Comparison of models</t>
   </si>
@@ -1182,6 +1182,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1215,9 +1218,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1529,7 +1529,7 @@
   <dimension ref="A1:U111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,73 +1550,73 @@
       <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="S8" s="51"/>
@@ -1632,10 +1632,10 @@
       <c r="D9" s="11">
         <v>2048</v>
       </c>
-      <c r="E9" s="64" t="s">
+      <c r="E9" s="65" t="s">
         <v>138</v>
       </c>
-      <c r="F9" s="65"/>
+      <c r="F9" s="66"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -1982,19 +1982,39 @@
       <c r="A17" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="19">
         <v>50</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="16"/>
+      <c r="C17" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="14">
+        <v>2260</v>
+      </c>
+      <c r="F17" s="14">
+        <v>0</v>
+      </c>
+      <c r="G17" s="14">
+        <v>5</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="K17" s="20">
+        <v>10</v>
+      </c>
+      <c r="L17" s="16" t="s">
+        <v>182</v>
+      </c>
       <c r="N17" s="48" t="s">
         <v>142</v>
       </c>
@@ -2008,21 +2028,41 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="18">
+        <v>91</v>
+      </c>
+      <c r="B18" s="19">
         <v>50</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="16"/>
+      <c r="C18" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="14">
+        <v>2260</v>
+      </c>
+      <c r="F18" s="14">
+        <v>0</v>
+      </c>
+      <c r="G18" s="14">
+        <v>5</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="K18" s="20">
+        <v>10</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>184</v>
+      </c>
       <c r="N18" s="48" t="s">
         <v>143</v>
       </c>
@@ -2035,22 +2075,6 @@
       <c r="U18" s="51"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="18">
-        <v>50</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="16"/>
       <c r="N19" s="48" t="s">
         <v>144</v>
       </c>
@@ -2062,23 +2086,7 @@
       <c r="T19" s="51"/>
       <c r="U19" s="51"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="18">
-        <v>25</v>
-      </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="16"/>
+    <row r="20" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N20" s="48" t="s">
         <v>145</v>
       </c>
@@ -2090,23 +2098,37 @@
       <c r="T20" s="51"/>
       <c r="U20" s="51"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="18">
-        <v>50</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="16"/>
+    <row r="21" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K21" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="L21" s="24" t="s">
+        <v>55</v>
+      </c>
       <c r="N21" s="52" t="s">
         <v>146</v>
       </c>
@@ -2120,21 +2142,35 @@
     </row>
     <row r="22" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B22" s="18">
-        <v>50</v>
-      </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="19">
+        <v>5000</v>
+      </c>
+      <c r="F22" s="19">
+        <v>0</v>
+      </c>
+      <c r="G22" s="19">
+        <v>5</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="15">
+        <v>16</v>
+      </c>
+      <c r="K22" s="20">
+        <v>10</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>177</v>
+      </c>
       <c r="N22" s="54" t="s">
         <v>147</v>
       </c>
@@ -2148,21 +2184,35 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B23" s="18">
-        <v>50</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="19">
+        <v>5000</v>
+      </c>
+      <c r="F23" s="19">
+        <v>0</v>
+      </c>
+      <c r="G23" s="19">
+        <v>5</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="K23" s="20">
+        <v>10</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>179</v>
+      </c>
       <c r="N23" s="51"/>
       <c r="O23" s="51"/>
       <c r="P23" s="51"/>
@@ -2174,40 +2224,34 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" s="19">
-        <v>50</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="14">
-        <v>2260</v>
-      </c>
-      <c r="F24" s="14">
+        <v>83</v>
+      </c>
+      <c r="B24" s="18">
+        <v>25</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="19">
+        <v>5000</v>
+      </c>
+      <c r="F24" s="18">
         <v>0</v>
       </c>
-      <c r="G24" s="14">
-        <v>5</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="I24" s="14" t="s">
+      <c r="G24" s="18">
+        <v>5</v>
+      </c>
+      <c r="I24" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="K24" s="20">
+      <c r="J24" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24" s="37">
         <v>10</v>
       </c>
-      <c r="L24" s="16" t="s">
-        <v>182</v>
+      <c r="L24" s="62" t="s">
+        <v>180</v>
       </c>
       <c r="N24" s="51"/>
       <c r="O24" s="51"/>
@@ -2218,43 +2262,17 @@
       <c r="T24" s="51"/>
       <c r="U24" s="51"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" s="19">
-        <v>50</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="14">
-        <v>2260</v>
-      </c>
-      <c r="F25" s="14">
-        <v>0</v>
-      </c>
-      <c r="G25" s="14">
-        <v>5</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="K25" s="20">
-        <v>10</v>
-      </c>
-      <c r="L25" s="16" t="s">
-        <v>184</v>
-      </c>
+    <row r="25" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="36"/>
       <c r="N25" s="51"/>
       <c r="O25" s="51"/>
       <c r="P25" s="51"/>
@@ -2294,162 +2312,20 @@
       <c r="T29" s="51"/>
       <c r="U29" s="51"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="Q30" s="51"/>
       <c r="R30" s="51"/>
       <c r="S30" s="51"/>
       <c r="T30" s="51"/>
       <c r="U30" s="51"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K31" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="L31" s="24" t="s">
-        <v>55</v>
-      </c>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="Q31" s="51"/>
       <c r="R31" s="51"/>
       <c r="S31" s="51"/>
       <c r="T31" s="51"/>
       <c r="U31" s="51"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="B32" s="18">
-        <v>25</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E32" s="19">
-        <v>5000</v>
-      </c>
-      <c r="F32" s="19">
-        <v>0</v>
-      </c>
-      <c r="G32" s="19">
-        <v>5</v>
-      </c>
-      <c r="I32" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J32" s="15">
-        <v>16</v>
-      </c>
-      <c r="K32" s="20">
-        <v>10</v>
-      </c>
-      <c r="L32" s="16" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="B33" s="18">
-        <v>25</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E33" s="19">
-        <v>5000</v>
-      </c>
-      <c r="F33" s="19">
-        <v>0</v>
-      </c>
-      <c r="G33" s="19">
-        <v>5</v>
-      </c>
-      <c r="I33" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J33" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="K33" s="20">
-        <v>10</v>
-      </c>
-      <c r="L33" s="16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="B34" s="18">
-        <v>50</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" s="19">
-        <v>5000</v>
-      </c>
-      <c r="F34" s="18">
-        <v>0</v>
-      </c>
-      <c r="G34" s="18">
-        <v>5</v>
-      </c>
-      <c r="I34" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="J34" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="K34" s="37">
-        <v>10</v>
-      </c>
-      <c r="L34" s="74" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" s="18">
-        <v>50</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="37"/>
-      <c r="L35" s="36"/>
-    </row>
     <row r="38" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="28" t="s">
@@ -2488,12 +2364,12 @@
       <c r="L39" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="O39" s="62" t="s">
+      <c r="O39" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="P39" s="62"/>
-      <c r="Q39" s="62"/>
-      <c r="R39" s="62"/>
+      <c r="P39" s="63"/>
+      <c r="Q39" s="63"/>
+      <c r="R39" s="63"/>
     </row>
     <row r="40" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14" t="s">
@@ -2512,10 +2388,10 @@
       <c r="J40" s="14"/>
       <c r="K40" s="14"/>
       <c r="L40" s="14"/>
-      <c r="O40" s="62"/>
-      <c r="P40" s="62"/>
-      <c r="Q40" s="62"/>
-      <c r="R40" s="62"/>
+      <c r="O40" s="63"/>
+      <c r="P40" s="63"/>
+      <c r="Q40" s="63"/>
+      <c r="R40" s="63"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
@@ -2534,16 +2410,16 @@
       <c r="J41" s="14"/>
       <c r="K41" s="14"/>
       <c r="L41" s="14"/>
-      <c r="O41" s="62"/>
-      <c r="P41" s="62"/>
-      <c r="Q41" s="62"/>
-      <c r="R41" s="62"/>
+      <c r="O41" s="63"/>
+      <c r="P41" s="63"/>
+      <c r="Q41" s="63"/>
+      <c r="R41" s="63"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="O42" s="62"/>
-      <c r="P42" s="62"/>
-      <c r="Q42" s="62"/>
-      <c r="R42" s="62"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="63"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="17"/>
@@ -2641,97 +2517,97 @@
       <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="70"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="70"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -2753,12 +2629,12 @@
       <c r="E11" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="65"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="66"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="O11" s="10"/>
@@ -3663,7 +3539,7 @@
   <dimension ref="A1:R35"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3684,77 +3560,77 @@
       <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="O4" s="71" t="s">
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="O4" s="72" t="s">
         <v>97</v>
       </c>
-      <c r="P4" s="71"/>
-      <c r="Q4" s="71"/>
-      <c r="R4" s="71"/>
+      <c r="P4" s="72"/>
+      <c r="Q4" s="72"/>
+      <c r="R4" s="72"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="O5" s="71"/>
-      <c r="P5" s="71"/>
-      <c r="Q5" s="71"/>
-      <c r="R5" s="71"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="72"/>
+      <c r="R5" s="72"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O6" s="71"/>
-      <c r="P6" s="71"/>
-      <c r="Q6" s="71"/>
-      <c r="R6" s="71"/>
+      <c r="O6" s="72"/>
+      <c r="P6" s="72"/>
+      <c r="Q6" s="72"/>
+      <c r="R6" s="72"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
@@ -3765,18 +3641,18 @@
       <c r="E7" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="65"/>
+      <c r="G7" s="66"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
-      <c r="O7" s="71"/>
-      <c r="P7" s="71"/>
-      <c r="Q7" s="71"/>
-      <c r="R7" s="71"/>
+      <c r="O7" s="72"/>
+      <c r="P7" s="72"/>
+      <c r="Q7" s="72"/>
+      <c r="R7" s="72"/>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
@@ -3901,12 +3777,12 @@
         <v>43</v>
       </c>
       <c r="N10" s="17"/>
-      <c r="O10" s="73" t="s">
+      <c r="O10" s="74" t="s">
         <v>105</v>
       </c>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
-      <c r="R10" s="73"/>
+      <c r="P10" s="74"/>
+      <c r="Q10" s="74"/>
+      <c r="R10" s="74"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
@@ -3949,10 +3825,10 @@
         <v>46</v>
       </c>
       <c r="N11" s="17"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="73"/>
-      <c r="R11" s="73"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
+      <c r="R11" s="74"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
@@ -3995,10 +3871,10 @@
         <v>48</v>
       </c>
       <c r="N12" s="17"/>
-      <c r="O12" s="73"/>
-      <c r="P12" s="73"/>
-      <c r="Q12" s="73"/>
-      <c r="R12" s="73"/>
+      <c r="O12" s="74"/>
+      <c r="P12" s="74"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="74"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
@@ -4088,12 +3964,12 @@
       <c r="N14" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="O14" s="70" t="s">
+      <c r="O14" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="P14" s="71"/>
-      <c r="Q14" s="71"/>
-      <c r="R14" s="71"/>
+      <c r="P14" s="72"/>
+      <c r="Q14" s="72"/>
+      <c r="R14" s="72"/>
     </row>
     <row r="15" spans="1:18" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34"/>
@@ -4110,10 +3986,10 @@
       <c r="L15" s="34"/>
       <c r="M15" s="34"/>
       <c r="N15" s="17"/>
-      <c r="O15" s="71"/>
-      <c r="P15" s="71"/>
-      <c r="Q15" s="71"/>
-      <c r="R15" s="71"/>
+      <c r="O15" s="72"/>
+      <c r="P15" s="72"/>
+      <c r="Q15" s="72"/>
+      <c r="R15" s="72"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
@@ -4156,10 +4032,10 @@
         <v>106</v>
       </c>
       <c r="N16" s="17"/>
-      <c r="O16" s="71"/>
-      <c r="P16" s="71"/>
-      <c r="Q16" s="71"/>
-      <c r="R16" s="71"/>
+      <c r="O16" s="72"/>
+      <c r="P16" s="72"/>
+      <c r="Q16" s="72"/>
+      <c r="R16" s="72"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
@@ -4202,10 +4078,10 @@
         <v>107</v>
       </c>
       <c r="N17" s="17"/>
-      <c r="O17" s="71"/>
-      <c r="P17" s="71"/>
-      <c r="Q17" s="71"/>
-      <c r="R17" s="71"/>
+      <c r="O17" s="72"/>
+      <c r="P17" s="72"/>
+      <c r="Q17" s="72"/>
+      <c r="R17" s="72"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
@@ -4248,10 +4124,10 @@
         <v>108</v>
       </c>
       <c r="N18" s="17"/>
-      <c r="O18" s="71"/>
-      <c r="P18" s="71"/>
-      <c r="Q18" s="71"/>
-      <c r="R18" s="71"/>
+      <c r="O18" s="72"/>
+      <c r="P18" s="72"/>
+      <c r="Q18" s="72"/>
+      <c r="R18" s="72"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
@@ -4294,10 +4170,10 @@
         <v>115</v>
       </c>
       <c r="N19" s="17"/>
-      <c r="O19" s="72"/>
-      <c r="P19" s="72"/>
-      <c r="Q19" s="72"/>
-      <c r="R19" s="72"/>
+      <c r="O19" s="73"/>
+      <c r="P19" s="73"/>
+      <c r="Q19" s="73"/>
+      <c r="R19" s="73"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
@@ -4631,37 +4507,37 @@
       <c r="A1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -4672,25 +4548,25 @@
       <c r="A4" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L8" s="22"/>
@@ -4704,10 +4580,10 @@
       <c r="D9" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="64" t="s">
+      <c r="E9" s="65" t="s">
         <v>150</v>
       </c>
-      <c r="F9" s="65"/>
+      <c r="F9" s="66"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>

</xml_diff>